<commit_message>
final analysis with correct age category
</commit_message>
<xml_diff>
--- a/data/V6-cyano-level-4-mod.xlsx
+++ b/data/V6-cyano-level-4-mod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucij\Documents\NGS Cyano analysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hrvoje\Documents\R-cyano-metabarcoding\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{818BE516-1160-4CBF-B771-50435BA62FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79A5685-0988-4FCA-92C0-C17BB49EE46A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -22,10 +22,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -861,29 +861,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8D664D-4B90-4EFF-AFB2-52533D929349}">
   <dimension ref="A1:AF391"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A325" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H356" sqref="H356"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="67" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -946,7 +946,7 @@
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -987,7 +987,7 @@
       <c r="AA2" s="1"/>
       <c r="AE2" s="1"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="AA3" s="1"/>
       <c r="AE3" s="1"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="AA4" s="1"/>
       <c r="AE4" s="1"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1110,7 +1110,7 @@
       <c r="AA5" s="1"/>
       <c r="AE5" s="1"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1151,7 +1151,7 @@
       <c r="AA6" s="1"/>
       <c r="AE6" s="1"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1192,7 +1192,7 @@
       <c r="AA7" s="1"/>
       <c r="AE7" s="1"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1233,7 +1233,7 @@
       <c r="AA8" s="1"/>
       <c r="AE8" s="1"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="AA9" s="1"/>
       <c r="AE9" s="1"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1315,7 +1315,7 @@
       <c r="AA10" s="1"/>
       <c r="AE10" s="1"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="AA11" s="1"/>
       <c r="AE11" s="1"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="AA12" s="1"/>
       <c r="AE12" s="1"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1438,7 +1438,7 @@
       <c r="AA13" s="1"/>
       <c r="AE13" s="1"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>136</v>
       </c>
@@ -1480,7 +1480,7 @@
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1542,7 +1542,7 @@
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1605,7 +1605,7 @@
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1668,7 +1668,7 @@
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1731,7 +1731,7 @@
       <c r="AD18" s="1"/>
       <c r="AE18" s="1"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1794,7 +1794,7 @@
       <c r="AD19" s="1"/>
       <c r="AE19" s="1"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1857,7 +1857,7 @@
       <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1920,7 +1920,7 @@
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1983,7 +1983,7 @@
       <c r="AD22" s="1"/>
       <c r="AE22" s="1"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -2093,7 +2093,7 @@
       <c r="AD24" s="1"/>
       <c r="AE24" s="1"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -2156,7 +2156,7 @@
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -2219,7 +2219,7 @@
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>136</v>
       </c>
@@ -2282,7 +2282,7 @@
       <c r="AD27" s="1"/>
       <c r="AE27" s="1"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
@@ -2342,7 +2342,7 @@
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -2402,7 +2402,7 @@
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -2465,7 +2465,7 @@
       <c r="AD30" s="1"/>
       <c r="AE30" s="1"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -2525,7 +2525,7 @@
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -2588,7 +2588,7 @@
       <c r="AD32" s="1"/>
       <c r="AE32" s="1"/>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -2651,7 +2651,7 @@
       <c r="AD33" s="1"/>
       <c r="AE33" s="1"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -2714,7 +2714,7 @@
       <c r="AD34" s="1"/>
       <c r="AE34" s="1"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>11</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>12</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>136</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>1</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>3</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>4</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>8</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>9</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>10</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>2</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>11</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>12</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>136</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>1</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>5</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>3</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>4</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>8</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>9</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>10</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>2</v>
       </c>
@@ -4030,7 +4030,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>11</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>12</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>6</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>136</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>1</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>5</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>7</v>
       </c>
@@ -4359,7 +4359,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>3</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>4</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>8</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>9</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>10</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>2</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>11</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>12</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>6</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>136</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>1</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>5</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>7</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>3</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>4</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>8</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>9</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>10</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>2</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>11</v>
       </c>
@@ -5269,7 +5269,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>12</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>6</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>136</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>1</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>5</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>7</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>3</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>4</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>8</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>9</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>10</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>2</v>
       </c>
@@ -5797,7 +5797,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>11</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>12</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>6</v>
       </c>
@@ -5929,7 +5929,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>136</v>
       </c>
@@ -5973,7 +5973,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>1</v>
       </c>
@@ -6017,7 +6017,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>5</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>7</v>
       </c>
@@ -6105,7 +6105,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>3</v>
       </c>
@@ -6149,7 +6149,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>4</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>8</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>9</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>10</v>
       </c>
@@ -6325,7 +6325,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>2</v>
       </c>
@@ -6369,7 +6369,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>11</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>12</v>
       </c>
@@ -6457,7 +6457,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>6</v>
       </c>
@@ -6501,7 +6501,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>136</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>1</v>
       </c>
@@ -6592,7 +6592,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>5</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>7</v>
       </c>
@@ -6686,7 +6686,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>3</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>4</v>
       </c>
@@ -6780,7 +6780,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>8</v>
       </c>
@@ -6827,7 +6827,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>9</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>10</v>
       </c>
@@ -6921,7 +6921,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>2</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>11</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>12</v>
       </c>
@@ -7062,7 +7062,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>6</v>
       </c>
@@ -7109,7 +7109,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>136</v>
       </c>
@@ -7156,7 +7156,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>1</v>
       </c>
@@ -7203,7 +7203,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>5</v>
       </c>
@@ -7250,7 +7250,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>7</v>
       </c>
@@ -7297,7 +7297,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>3</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>4</v>
       </c>
@@ -7391,7 +7391,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>8</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>9</v>
       </c>
@@ -7485,7 +7485,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>10</v>
       </c>
@@ -7532,7 +7532,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>2</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>11</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>12</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>6</v>
       </c>
@@ -7720,7 +7720,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>136</v>
       </c>
@@ -7767,7 +7767,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>1</v>
       </c>
@@ -7814,7 +7814,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>5</v>
       </c>
@@ -7861,7 +7861,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>7</v>
       </c>
@@ -7908,7 +7908,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>3</v>
       </c>
@@ -7955,7 +7955,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>4</v>
       </c>
@@ -8002,7 +8002,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>8</v>
       </c>
@@ -8049,7 +8049,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>9</v>
       </c>
@@ -8096,7 +8096,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>10</v>
       </c>
@@ -8143,7 +8143,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>2</v>
       </c>
@@ -8190,7 +8190,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>11</v>
       </c>
@@ -8237,7 +8237,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>12</v>
       </c>
@@ -8284,7 +8284,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>6</v>
       </c>
@@ -8331,7 +8331,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>136</v>
       </c>
@@ -8378,7 +8378,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>1</v>
       </c>
@@ -8425,7 +8425,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>5</v>
       </c>
@@ -8472,7 +8472,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>7</v>
       </c>
@@ -8519,7 +8519,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>3</v>
       </c>
@@ -8566,7 +8566,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>4</v>
       </c>
@@ -8613,7 +8613,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>8</v>
       </c>
@@ -8660,7 +8660,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>9</v>
       </c>
@@ -8707,7 +8707,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>10</v>
       </c>
@@ -8754,7 +8754,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>2</v>
       </c>
@@ -8801,7 +8801,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>11</v>
       </c>
@@ -8848,7 +8848,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>12</v>
       </c>
@@ -8895,7 +8895,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>6</v>
       </c>
@@ -8942,7 +8942,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>136</v>
       </c>
@@ -8989,7 +8989,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>1</v>
       </c>
@@ -9036,7 +9036,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>5</v>
       </c>
@@ -9083,7 +9083,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>7</v>
       </c>
@@ -9130,7 +9130,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>3</v>
       </c>
@@ -9177,7 +9177,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>4</v>
       </c>
@@ -9224,7 +9224,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>8</v>
       </c>
@@ -9271,7 +9271,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>9</v>
       </c>
@@ -9318,7 +9318,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>10</v>
       </c>
@@ -9365,7 +9365,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>2</v>
       </c>
@@ -9412,7 +9412,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>11</v>
       </c>
@@ -9459,7 +9459,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>12</v>
       </c>
@@ -9506,7 +9506,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>6</v>
       </c>
@@ -9553,7 +9553,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>136</v>
       </c>
@@ -9600,7 +9600,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>1</v>
       </c>
@@ -9647,7 +9647,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>5</v>
       </c>
@@ -9694,7 +9694,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>7</v>
       </c>
@@ -9741,7 +9741,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>3</v>
       </c>
@@ -9788,7 +9788,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>4</v>
       </c>
@@ -9835,7 +9835,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>8</v>
       </c>
@@ -9882,7 +9882,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>9</v>
       </c>
@@ -9929,7 +9929,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>10</v>
       </c>
@@ -9976,7 +9976,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>2</v>
       </c>
@@ -10023,7 +10023,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>11</v>
       </c>
@@ -10070,7 +10070,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>12</v>
       </c>
@@ -10117,7 +10117,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>6</v>
       </c>
@@ -10164,7 +10164,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>136</v>
       </c>
@@ -10211,7 +10211,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>1</v>
       </c>
@@ -10234,7 +10234,7 @@
         <v>87</v>
       </c>
       <c r="H197" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I197" s="1">
         <v>55</v>
@@ -10258,7 +10258,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>5</v>
       </c>
@@ -10281,7 +10281,7 @@
         <v>87</v>
       </c>
       <c r="H198" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I198" s="1">
         <v>55</v>
@@ -10305,7 +10305,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>7</v>
       </c>
@@ -10328,7 +10328,7 @@
         <v>87</v>
       </c>
       <c r="H199" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I199" s="1">
         <v>55</v>
@@ -10352,7 +10352,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>3</v>
       </c>
@@ -10375,7 +10375,7 @@
         <v>87</v>
       </c>
       <c r="H200" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I200" s="1">
         <v>55</v>
@@ -10399,7 +10399,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>4</v>
       </c>
@@ -10422,7 +10422,7 @@
         <v>87</v>
       </c>
       <c r="H201" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I201" s="1">
         <v>55</v>
@@ -10446,7 +10446,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>8</v>
       </c>
@@ -10469,7 +10469,7 @@
         <v>87</v>
       </c>
       <c r="H202" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I202" s="1">
         <v>55</v>
@@ -10493,7 +10493,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>9</v>
       </c>
@@ -10516,7 +10516,7 @@
         <v>87</v>
       </c>
       <c r="H203" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I203" s="1">
         <v>55</v>
@@ -10540,7 +10540,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>10</v>
       </c>
@@ -10563,7 +10563,7 @@
         <v>87</v>
       </c>
       <c r="H204" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I204" s="1">
         <v>55</v>
@@ -10587,7 +10587,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>2</v>
       </c>
@@ -10610,7 +10610,7 @@
         <v>87</v>
       </c>
       <c r="H205" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I205" s="1">
         <v>55</v>
@@ -10634,7 +10634,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>11</v>
       </c>
@@ -10657,7 +10657,7 @@
         <v>87</v>
       </c>
       <c r="H206" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I206" s="1">
         <v>55</v>
@@ -10681,7 +10681,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>12</v>
       </c>
@@ -10704,7 +10704,7 @@
         <v>87</v>
       </c>
       <c r="H207" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I207" s="1">
         <v>55</v>
@@ -10728,7 +10728,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>6</v>
       </c>
@@ -10751,7 +10751,7 @@
         <v>87</v>
       </c>
       <c r="H208" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I208" s="1">
         <v>55</v>
@@ -10775,7 +10775,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>136</v>
       </c>
@@ -10798,7 +10798,7 @@
         <v>87</v>
       </c>
       <c r="H209" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I209" s="1">
         <v>55</v>
@@ -10822,7 +10822,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>1</v>
       </c>
@@ -10869,7 +10869,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>5</v>
       </c>
@@ -10916,7 +10916,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>7</v>
       </c>
@@ -10963,7 +10963,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>3</v>
       </c>
@@ -11010,7 +11010,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>4</v>
       </c>
@@ -11057,7 +11057,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>8</v>
       </c>
@@ -11104,7 +11104,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>9</v>
       </c>
@@ -11151,7 +11151,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>10</v>
       </c>
@@ -11198,7 +11198,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>2</v>
       </c>
@@ -11245,7 +11245,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>11</v>
       </c>
@@ -11292,7 +11292,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>12</v>
       </c>
@@ -11339,7 +11339,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>6</v>
       </c>
@@ -11386,7 +11386,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>136</v>
       </c>
@@ -11433,7 +11433,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>1</v>
       </c>
@@ -11480,7 +11480,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>5</v>
       </c>
@@ -11527,7 +11527,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>7</v>
       </c>
@@ -11574,7 +11574,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>3</v>
       </c>
@@ -11621,7 +11621,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>4</v>
       </c>
@@ -11668,7 +11668,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>8</v>
       </c>
@@ -11715,7 +11715,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>9</v>
       </c>
@@ -11762,7 +11762,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>10</v>
       </c>
@@ -11809,7 +11809,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>2</v>
       </c>
@@ -11856,7 +11856,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>11</v>
       </c>
@@ -11903,7 +11903,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>12</v>
       </c>
@@ -11950,7 +11950,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>6</v>
       </c>
@@ -11997,7 +11997,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>136</v>
       </c>
@@ -12044,7 +12044,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>1</v>
       </c>
@@ -12091,7 +12091,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>5</v>
       </c>
@@ -12138,7 +12138,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>7</v>
       </c>
@@ -12185,7 +12185,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>3</v>
       </c>
@@ -12232,7 +12232,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>4</v>
       </c>
@@ -12279,7 +12279,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>8</v>
       </c>
@@ -12326,7 +12326,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>9</v>
       </c>
@@ -12373,7 +12373,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>10</v>
       </c>
@@ -12420,7 +12420,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>2</v>
       </c>
@@ -12467,7 +12467,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>11</v>
       </c>
@@ -12514,7 +12514,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>12</v>
       </c>
@@ -12561,7 +12561,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>6</v>
       </c>
@@ -12608,7 +12608,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>136</v>
       </c>
@@ -12655,7 +12655,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>1</v>
       </c>
@@ -12702,7 +12702,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>5</v>
       </c>
@@ -12749,7 +12749,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
         <v>7</v>
       </c>
@@ -12796,7 +12796,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>3</v>
       </c>
@@ -12843,7 +12843,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>4</v>
       </c>
@@ -12890,7 +12890,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>8</v>
       </c>
@@ -12937,7 +12937,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>9</v>
       </c>
@@ -12984,7 +12984,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>10</v>
       </c>
@@ -13031,7 +13031,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="257" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
         <v>2</v>
       </c>
@@ -13078,7 +13078,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="258" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
         <v>11</v>
       </c>
@@ -13125,7 +13125,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="259" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>12</v>
       </c>
@@ -13172,7 +13172,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="260" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
         <v>6</v>
       </c>
@@ -13219,7 +13219,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="261" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>136</v>
       </c>
@@ -13266,7 +13266,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="262" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
         <v>1</v>
       </c>
@@ -13313,7 +13313,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="263" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>5</v>
       </c>
@@ -13360,7 +13360,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="264" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>7</v>
       </c>
@@ -13407,7 +13407,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="265" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>3</v>
       </c>
@@ -13454,7 +13454,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="266" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>4</v>
       </c>
@@ -13501,7 +13501,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="267" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
         <v>8</v>
       </c>
@@ -13548,7 +13548,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="268" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>9</v>
       </c>
@@ -13595,7 +13595,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="269" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>10</v>
       </c>
@@ -13642,7 +13642,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="270" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
         <v>2</v>
       </c>
@@ -13689,7 +13689,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="271" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
         <v>11</v>
       </c>
@@ -13736,7 +13736,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="272" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
         <v>12</v>
       </c>
@@ -13783,7 +13783,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
         <v>6</v>
       </c>
@@ -13830,7 +13830,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>136</v>
       </c>
@@ -13877,7 +13877,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="275" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
         <v>1</v>
       </c>
@@ -13915,7 +13915,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="276" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>5</v>
       </c>
@@ -13953,7 +13953,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="277" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
         <v>7</v>
       </c>
@@ -13991,7 +13991,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="278" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>3</v>
       </c>
@@ -14029,7 +14029,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="279" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
         <v>4</v>
       </c>
@@ -14067,7 +14067,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>8</v>
       </c>
@@ -14105,7 +14105,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
         <v>9</v>
       </c>
@@ -14143,7 +14143,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="282" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
         <v>10</v>
       </c>
@@ -14181,7 +14181,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="283" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
         <v>2</v>
       </c>
@@ -14219,7 +14219,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="284" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
         <v>11</v>
       </c>
@@ -14257,7 +14257,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="285" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="s">
         <v>12</v>
       </c>
@@ -14295,7 +14295,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="286" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
         <v>6</v>
       </c>
@@ -14333,7 +14333,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="287" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="s">
         <v>136</v>
       </c>
@@ -14371,7 +14371,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="288" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
         <v>1</v>
       </c>
@@ -14418,7 +14418,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="289" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
         <v>5</v>
       </c>
@@ -14465,7 +14465,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="290" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
         <v>7</v>
       </c>
@@ -14512,7 +14512,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="291" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A291" s="1" t="s">
         <v>3</v>
       </c>
@@ -14559,7 +14559,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="292" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
         <v>4</v>
       </c>
@@ -14606,7 +14606,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="293" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="s">
         <v>8</v>
       </c>
@@ -14653,7 +14653,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="294" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="s">
         <v>9</v>
       </c>
@@ -14700,7 +14700,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="295" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A295" s="1" t="s">
         <v>10</v>
       </c>
@@ -14747,7 +14747,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="296" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
         <v>2</v>
       </c>
@@ -14794,7 +14794,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="297" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A297" s="1" t="s">
         <v>11</v>
       </c>
@@ -14841,7 +14841,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="298" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
         <v>12</v>
       </c>
@@ -14888,7 +14888,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="299" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A299" s="1" t="s">
         <v>6</v>
       </c>
@@ -14935,7 +14935,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="300" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
         <v>136</v>
       </c>
@@ -14982,7 +14982,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="301" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A301" s="1" t="s">
         <v>1</v>
       </c>
@@ -15020,7 +15020,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="302" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
         <v>5</v>
       </c>
@@ -15058,7 +15058,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="303" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A303" s="1" t="s">
         <v>7</v>
       </c>
@@ -15096,7 +15096,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="304" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="s">
         <v>3</v>
       </c>
@@ -15134,7 +15134,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="305" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A305" s="1" t="s">
         <v>4</v>
       </c>
@@ -15172,7 +15172,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="306" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
         <v>8</v>
       </c>
@@ -15210,7 +15210,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="307" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A307" s="1" t="s">
         <v>9</v>
       </c>
@@ -15248,7 +15248,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="308" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
         <v>10</v>
       </c>
@@ -15286,7 +15286,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="309" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A309" s="1" t="s">
         <v>2</v>
       </c>
@@ -15324,7 +15324,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="310" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
         <v>11</v>
       </c>
@@ -15362,7 +15362,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="311" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A311" s="1" t="s">
         <v>12</v>
       </c>
@@ -15400,7 +15400,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="312" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
         <v>6</v>
       </c>
@@ -15438,7 +15438,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="313" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A313" s="1" t="s">
         <v>136</v>
       </c>
@@ -15476,7 +15476,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="314" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A314" s="1" t="s">
         <v>1</v>
       </c>
@@ -15523,7 +15523,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="315" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A315" s="1" t="s">
         <v>5</v>
       </c>
@@ -15570,7 +15570,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="316" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A316" s="1" t="s">
         <v>7</v>
       </c>
@@ -15617,7 +15617,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="317" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A317" s="1" t="s">
         <v>3</v>
       </c>
@@ -15664,7 +15664,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="318" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A318" s="1" t="s">
         <v>4</v>
       </c>
@@ -15711,7 +15711,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="319" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A319" s="1" t="s">
         <v>8</v>
       </c>
@@ -15758,7 +15758,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="320" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A320" s="1" t="s">
         <v>9</v>
       </c>
@@ -15805,7 +15805,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="321" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A321" s="1" t="s">
         <v>10</v>
       </c>
@@ -15852,7 +15852,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="322" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
         <v>2</v>
       </c>
@@ -15899,7 +15899,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="323" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A323" s="1" t="s">
         <v>11</v>
       </c>
@@ -15946,7 +15946,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="324" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
         <v>12</v>
       </c>
@@ -15993,7 +15993,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="325" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
         <v>6</v>
       </c>
@@ -16040,7 +16040,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="326" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
         <v>136</v>
       </c>
@@ -16087,7 +16087,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="327" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A327" s="1" t="s">
         <v>1</v>
       </c>
@@ -16134,7 +16134,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="328" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A328" s="1" t="s">
         <v>5</v>
       </c>
@@ -16181,7 +16181,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="329" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A329" s="1" t="s">
         <v>7</v>
       </c>
@@ -16228,7 +16228,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="330" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A330" s="1" t="s">
         <v>3</v>
       </c>
@@ -16275,7 +16275,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="331" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A331" s="1" t="s">
         <v>4</v>
       </c>
@@ -16322,7 +16322,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="332" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A332" s="1" t="s">
         <v>8</v>
       </c>
@@ -16369,7 +16369,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="333" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A333" s="1" t="s">
         <v>9</v>
       </c>
@@ -16416,7 +16416,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="334" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A334" s="1" t="s">
         <v>10</v>
       </c>
@@ -16463,7 +16463,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="335" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A335" s="1" t="s">
         <v>2</v>
       </c>
@@ -16510,7 +16510,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="336" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A336" s="1" t="s">
         <v>11</v>
       </c>
@@ -16557,7 +16557,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="337" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A337" s="1" t="s">
         <v>12</v>
       </c>
@@ -16604,7 +16604,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="338" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A338" s="1" t="s">
         <v>6</v>
       </c>
@@ -16651,7 +16651,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="339" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A339" s="1" t="s">
         <v>136</v>
       </c>
@@ -16698,7 +16698,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="340" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
         <v>1</v>
       </c>
@@ -16721,7 +16721,7 @@
         <v>126</v>
       </c>
       <c r="H340" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I340" s="1">
         <v>52</v>
@@ -16745,7 +16745,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="341" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A341" s="1" t="s">
         <v>5</v>
       </c>
@@ -16768,7 +16768,7 @@
         <v>126</v>
       </c>
       <c r="H341" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I341" s="1">
         <v>52</v>
@@ -16792,7 +16792,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="342" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A342" s="1" t="s">
         <v>7</v>
       </c>
@@ -16815,7 +16815,7 @@
         <v>126</v>
       </c>
       <c r="H342" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I342" s="1">
         <v>52</v>
@@ -16839,7 +16839,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="343" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A343" s="1" t="s">
         <v>3</v>
       </c>
@@ -16862,7 +16862,7 @@
         <v>126</v>
       </c>
       <c r="H343" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I343" s="1">
         <v>52</v>
@@ -16886,7 +16886,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="344" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A344" s="1" t="s">
         <v>4</v>
       </c>
@@ -16909,7 +16909,7 @@
         <v>126</v>
       </c>
       <c r="H344" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I344" s="1">
         <v>52</v>
@@ -16933,7 +16933,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="345" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A345" s="1" t="s">
         <v>8</v>
       </c>
@@ -16956,7 +16956,7 @@
         <v>126</v>
       </c>
       <c r="H345" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I345" s="1">
         <v>52</v>
@@ -16980,7 +16980,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="346" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A346" s="1" t="s">
         <v>9</v>
       </c>
@@ -17003,7 +17003,7 @@
         <v>126</v>
       </c>
       <c r="H346" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I346" s="1">
         <v>52</v>
@@ -17027,7 +17027,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="347" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A347" s="1" t="s">
         <v>10</v>
       </c>
@@ -17050,7 +17050,7 @@
         <v>126</v>
       </c>
       <c r="H347" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I347" s="1">
         <v>52</v>
@@ -17074,7 +17074,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="348" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A348" s="1" t="s">
         <v>2</v>
       </c>
@@ -17097,7 +17097,7 @@
         <v>126</v>
       </c>
       <c r="H348" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I348" s="1">
         <v>52</v>
@@ -17121,7 +17121,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="349" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A349" s="1" t="s">
         <v>11</v>
       </c>
@@ -17144,7 +17144,7 @@
         <v>126</v>
       </c>
       <c r="H349" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I349" s="1">
         <v>52</v>
@@ -17168,7 +17168,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="350" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A350" s="1" t="s">
         <v>12</v>
       </c>
@@ -17191,7 +17191,7 @@
         <v>126</v>
       </c>
       <c r="H350" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I350" s="1">
         <v>52</v>
@@ -17215,7 +17215,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="351" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A351" s="1" t="s">
         <v>6</v>
       </c>
@@ -17238,7 +17238,7 @@
         <v>126</v>
       </c>
       <c r="H351" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I351" s="1">
         <v>52</v>
@@ -17262,7 +17262,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="352" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
         <v>136</v>
       </c>
@@ -17285,7 +17285,7 @@
         <v>126</v>
       </c>
       <c r="H352" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="I352" s="1">
         <v>52</v>
@@ -17309,7 +17309,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="353" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A353" s="1" t="s">
         <v>1</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="354" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
         <v>5</v>
       </c>
@@ -17403,7 +17403,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="355" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A355" s="1" t="s">
         <v>7</v>
       </c>
@@ -17450,7 +17450,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="356" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
         <v>3</v>
       </c>
@@ -17497,7 +17497,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="357" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A357" s="1" t="s">
         <v>4</v>
       </c>
@@ -17544,7 +17544,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="358" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A358" s="1" t="s">
         <v>8</v>
       </c>
@@ -17591,7 +17591,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="359" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A359" s="1" t="s">
         <v>9</v>
       </c>
@@ -17638,7 +17638,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="360" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A360" s="1" t="s">
         <v>10</v>
       </c>
@@ -17685,7 +17685,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="361" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A361" s="1" t="s">
         <v>2</v>
       </c>
@@ -17732,7 +17732,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="362" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A362" s="1" t="s">
         <v>11</v>
       </c>
@@ -17779,7 +17779,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="363" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A363" s="1" t="s">
         <v>12</v>
       </c>
@@ -17826,7 +17826,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="364" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A364" s="1" t="s">
         <v>6</v>
       </c>
@@ -17873,7 +17873,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="365" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A365" s="1" t="s">
         <v>136</v>
       </c>
@@ -17920,7 +17920,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="366" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A366" s="1" t="s">
         <v>1</v>
       </c>
@@ -17967,7 +17967,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="367" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A367" s="1" t="s">
         <v>5</v>
       </c>
@@ -18014,7 +18014,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="368" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A368" s="1" t="s">
         <v>7</v>
       </c>
@@ -18061,7 +18061,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="369" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A369" s="1" t="s">
         <v>3</v>
       </c>
@@ -18108,7 +18108,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="370" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A370" s="1" t="s">
         <v>4</v>
       </c>
@@ -18155,7 +18155,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="371" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A371" s="1" t="s">
         <v>8</v>
       </c>
@@ -18202,7 +18202,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="372" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A372" s="1" t="s">
         <v>9</v>
       </c>
@@ -18249,7 +18249,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="373" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A373" s="1" t="s">
         <v>10</v>
       </c>
@@ -18296,7 +18296,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="374" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A374" s="1" t="s">
         <v>2</v>
       </c>
@@ -18343,7 +18343,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="375" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A375" s="1" t="s">
         <v>11</v>
       </c>
@@ -18390,7 +18390,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="376" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A376" s="1" t="s">
         <v>12</v>
       </c>
@@ -18437,7 +18437,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="377" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A377" s="1" t="s">
         <v>6</v>
       </c>
@@ -18484,7 +18484,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="378" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A378" s="1" t="s">
         <v>136</v>
       </c>
@@ -18531,7 +18531,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="379" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A379" s="1" t="s">
         <v>1</v>
       </c>
@@ -18569,7 +18569,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="380" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A380" s="1" t="s">
         <v>5</v>
       </c>
@@ -18607,7 +18607,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="381" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A381" s="1" t="s">
         <v>7</v>
       </c>
@@ -18645,7 +18645,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="382" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A382" s="1" t="s">
         <v>3</v>
       </c>
@@ -18683,7 +18683,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="383" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A383" s="1" t="s">
         <v>4</v>
       </c>
@@ -18721,7 +18721,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="384" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A384" s="1" t="s">
         <v>8</v>
       </c>
@@ -18759,7 +18759,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="385" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A385" s="1" t="s">
         <v>9</v>
       </c>
@@ -18797,7 +18797,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="386" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A386" s="1" t="s">
         <v>10</v>
       </c>
@@ -18835,7 +18835,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="387" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A387" s="1" t="s">
         <v>2</v>
       </c>
@@ -18873,7 +18873,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="388" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A388" s="1" t="s">
         <v>11</v>
       </c>
@@ -18911,7 +18911,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="389" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A389" s="1" t="s">
         <v>12</v>
       </c>
@@ -18949,7 +18949,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="390" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A390" s="1" t="s">
         <v>6</v>
       </c>
@@ -18987,7 +18987,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="391" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A391" s="1" t="s">
         <v>136</v>
       </c>
@@ -19026,7 +19026,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF22">
+  <sortState ref="A2:AF22">
     <sortCondition descending="1" ref="AF2:AF22"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>